<commit_message>
inclusão dos gráficos após 100 casos para SP
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -59539,10 +59539,10 @@
         <v>2095</v>
       </c>
       <c r="F2043" t="n">
-        <v>66.0</v>
+        <v>165.0</v>
       </c>
       <c r="G2043" t="n">
-        <v>924.0</v>
+        <v>1023.0</v>
       </c>
       <c r="H2043" t="n">
         <v>17.0</v>
@@ -59747,13 +59747,13 @@
         <v>2095</v>
       </c>
       <c r="F2051" t="n">
-        <v>98.0</v>
+        <v>174.0</v>
       </c>
       <c r="G2051" t="n">
-        <v>4697.0</v>
+        <v>4773.0</v>
       </c>
       <c r="H2051" t="n">
-        <v>200.0</v>
+        <v>212.0</v>
       </c>
     </row>
     <row r="2052">
@@ -59929,10 +59929,10 @@
         <v>2095</v>
       </c>
       <c r="F2058" t="n">
-        <v>162.0</v>
+        <v>161.0</v>
       </c>
       <c r="G2058" t="n">
-        <v>2592.0</v>
+        <v>2591.0</v>
       </c>
       <c r="H2058" t="n">
         <v>52.0</v>
@@ -59955,13 +59955,13 @@
         <v>2095</v>
       </c>
       <c r="F2059" t="n">
-        <v>14189.0</v>
+        <v>14363.0</v>
       </c>
       <c r="G2059" t="n">
-        <v>365754.0</v>
+        <v>365928.0</v>
       </c>
       <c r="H2059" t="n">
-        <v>22843.0</v>
+        <v>22855.0</v>
       </c>
     </row>
     <row r="2060">
@@ -60267,7 +60267,7 @@
         <v>2095</v>
       </c>
       <c r="F2071" t="n">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
       <c r="G2071" t="n">
         <v>1023.0</v>
@@ -60475,7 +60475,7 @@
         <v>2095</v>
       </c>
       <c r="F2079" t="n">
-        <v>77.0</v>
+        <v>1.0</v>
       </c>
       <c r="G2079" t="n">
         <v>4774.0</v>
@@ -60527,10 +60527,10 @@
         <v>2095</v>
       </c>
       <c r="F2081" t="n">
-        <v>75.0</v>
+        <v>125.0</v>
       </c>
       <c r="G2081" t="n">
-        <v>2514.0</v>
+        <v>2564.0</v>
       </c>
       <c r="H2081" t="n">
         <v>86.0</v>
@@ -60660,7 +60660,7 @@
         <v>105.0</v>
       </c>
       <c r="G2086" t="n">
-        <v>2697.0</v>
+        <v>2696.0</v>
       </c>
       <c r="H2086" t="n">
         <v>58.0</v>
@@ -60683,10 +60683,10 @@
         <v>2095</v>
       </c>
       <c r="F2087" t="n">
-        <v>12211.0</v>
+        <v>12086.0</v>
       </c>
       <c r="G2087" t="n">
-        <v>377965.0</v>
+        <v>378014.0</v>
       </c>
       <c r="H2087" t="n">
         <v>23580.0</v>

</xml_diff>

<commit_message>
Inclusão dos Heatmaps TEM QUE USAR PLOTLY V3.8.0
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -61429,7 +61429,7 @@
         <v>2583.0</v>
       </c>
       <c r="H2109" t="n">
-        <v>710.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="2110">
@@ -61585,7 +61585,7 @@
         <v>393542.0</v>
       </c>
       <c r="H2115" t="n">
-        <v>25176.0</v>
+        <v>24568.0</v>
       </c>
     </row>
     <row r="2116">
@@ -61923,7 +61923,7 @@
         <v>1909.0</v>
       </c>
       <c r="H2128" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="2129">
@@ -62313,7 +62313,7 @@
         <v>414740.0</v>
       </c>
       <c r="H2143" t="n">
-        <v>25698.0</v>
+        <v>25699.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Inclusão dos Heatmaps TEM QUE USAR PLOTLY V3.8.0"
This reverts commit 44b43ae632177b0d75819f1730643020d0f5ff87.
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -61429,7 +61429,7 @@
         <v>2583.0</v>
       </c>
       <c r="H2109" t="n">
-        <v>102.0</v>
+        <v>710.0</v>
       </c>
     </row>
     <row r="2110">
@@ -61585,7 +61585,7 @@
         <v>393542.0</v>
       </c>
       <c r="H2115" t="n">
-        <v>24568.0</v>
+        <v>25176.0</v>
       </c>
     </row>
     <row r="2116">
@@ -61923,7 +61923,7 @@
         <v>1909.0</v>
       </c>
       <c r="H2128" t="n">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="2129">
@@ -62313,7 +62313,7 @@
         <v>414740.0</v>
       </c>
       <c r="H2143" t="n">
-        <v>25699.0</v>
+        <v>25698.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Inclusão dos Heatmaps TEM QUE USAR PLOTLY V3.8.0""
This reverts commit 1f7c07aff107714ec314c596213e263ed05724cb.
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -61429,7 +61429,7 @@
         <v>2583.0</v>
       </c>
       <c r="H2109" t="n">
-        <v>710.0</v>
+        <v>102.0</v>
       </c>
     </row>
     <row r="2110">
@@ -61585,7 +61585,7 @@
         <v>393542.0</v>
       </c>
       <c r="H2115" t="n">
-        <v>25176.0</v>
+        <v>24568.0</v>
       </c>
     </row>
     <row r="2116">
@@ -61923,7 +61923,7 @@
         <v>1909.0</v>
       </c>
       <c r="H2128" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="2129">
@@ -62313,7 +62313,7 @@
         <v>414740.0</v>
       </c>
       <c r="H2143" t="n">
-        <v>25698.0</v>
+        <v>25699.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inclusão mortes , dados do MS
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -66717,7 +66717,7 @@
         <v>38174.0</v>
       </c>
       <c r="H2293" t="n">
-        <v>997.0</v>
+        <v>1028.0</v>
       </c>
     </row>
     <row r="2294">
@@ -66795,7 +66795,7 @@
         <v>2817.0</v>
       </c>
       <c r="H2296" t="n">
-        <v>70.0</v>
+        <v>75.0</v>
       </c>
     </row>
     <row r="2297">
@@ -67023,13 +67023,13 @@
         <v>2319</v>
       </c>
       <c r="F2305" t="n">
-        <v>158.0</v>
+        <v>451.0</v>
       </c>
       <c r="G2305" t="n">
-        <v>3850.0</v>
+        <v>4143.0</v>
       </c>
       <c r="H2305" t="n">
-        <v>120.0</v>
+        <v>124.0</v>
       </c>
     </row>
     <row r="2306">
@@ -67179,13 +67179,13 @@
         <v>2319</v>
       </c>
       <c r="F2311" t="n">
-        <v>30906.0</v>
+        <v>31199.0</v>
       </c>
       <c r="G2311" t="n">
-        <v>561471.0</v>
+        <v>561764.0</v>
       </c>
       <c r="H2311" t="n">
-        <v>31398.0</v>
+        <v>31438.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcao na coleta do rawdata
</commit_message>
<xml_diff>
--- a/docs/excel_base.xlsx
+++ b/docs/excel_base.xlsx
@@ -84445,10 +84445,10 @@
         <v>2935</v>
       </c>
       <c r="F2904" t="n">
-        <v>2846.0</v>
+        <v>2847.0</v>
       </c>
       <c r="G2904" t="n">
-        <v>51931.0</v>
+        <v>51932.0</v>
       </c>
       <c r="H2904" t="n">
         <v>1541.0</v>
@@ -85043,10 +85043,10 @@
         <v>2935</v>
       </c>
       <c r="F2927" t="n">
-        <v>39536.0</v>
+        <v>39537.0</v>
       </c>
       <c r="G2927" t="n">
-        <v>1193761.0</v>
+        <v>1193762.0</v>
       </c>
       <c r="H2927" t="n">
         <v>53897.0</v>

</xml_diff>